<commit_message>
✨ Adiciona script de diagnóstico de qualidade dos textos limpos
</commit_message>
<xml_diff>
--- a/controle_documentos.xlsx
+++ b/controle_documentos.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isisi\Documents\IAVS_PROJETO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49650CF-41EF-4649-B19F-05E2889BDCB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB21F8A7-9D54-47FC-8551-0E6CC1708FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7495ED94-32AF-4984-90A6-A4DB1F4E4893}"/>
   </bookViews>
   <sheets>
     <sheet name="docs" sheetId="2" r:id="rId1"/>
-    <sheet name="fontes_complementares" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">docs!$A$1:$J$65</definedName>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="379">
   <si>
     <t>ID</t>
   </si>
@@ -761,129 +760,6 @@
   </si>
   <si>
     <t>Apresenta diretrizes laboratoriais atualizadas para o diagnóstico da sífilis, com ênfase em algoritmos treponêmicos e não treponêmicos, interpretação de resultados, fluxogramas clínico-laboratoriais e recomendações específicas para gestantes, puérperas e recém-nascidos.</t>
-  </si>
-  <si>
-    <t>Conteúdo Útil</t>
-  </si>
-  <si>
-    <t>Doenças/Tema</t>
-  </si>
-  <si>
-    <t>Observações</t>
-  </si>
-  <si>
-    <t>OPAS/OMS</t>
-  </si>
-  <si>
-    <t>Notícias Técnicas</t>
-  </si>
-  <si>
-    <t>Atualizações frequentes sobre surtos, novas recomendações técnicas</t>
-  </si>
-  <si>
-    <t>Diversas doenças emergentes</t>
-  </si>
-  <si>
-    <t>Boletins com abordagem técnica e operacional</t>
-  </si>
-  <si>
-    <t>Pode conter atualizações de protocolos</t>
-  </si>
-  <si>
-    <t>Ministério da Saúde</t>
-  </si>
-  <si>
-    <t>Portal por doenças</t>
-  </si>
-  <si>
-    <t>Links diretos por ordem alfabética de temas</t>
-  </si>
-  <si>
-    <t>Zoonoses, arboviroses, HIV, etc.</t>
-  </si>
-  <si>
-    <t>Acesso rápido a documentos específicos por tema</t>
-  </si>
-  <si>
-    <t>Anvisa</t>
-  </si>
-  <si>
-    <t>https://www.gov.br/anvisa/pt-br/assuntos/noticias-anvisa</t>
-  </si>
-  <si>
-    <t>Notícias Regulatórias</t>
-  </si>
-  <si>
-    <t>Alertas e novas orientações sobre medicamentos e vigilância sanitária</t>
-  </si>
-  <si>
-    <t>Segurança do paciente, surtos</t>
-  </si>
-  <si>
-    <t>Conteúdo dinâmico e complementar</t>
-  </si>
-  <si>
-    <t>Fiocruz</t>
-  </si>
-  <si>
-    <t>Publicações Técnicas</t>
-  </si>
-  <si>
-    <t>Guias, recomendações e estudos técnicos</t>
-  </si>
-  <si>
-    <t>Saúde Pública em geral</t>
-  </si>
-  <si>
-    <t>Produções recentes que não estão listadas nos seus PDFs</t>
-  </si>
-  <si>
-    <t>CDC</t>
-  </si>
-  <si>
-    <t>Conteúdo Técnico</t>
-  </si>
-  <si>
-    <t>Protocolos e fichas técnicas por doença</t>
-  </si>
-  <si>
-    <t>Dengue, Influenza, etc.</t>
-  </si>
-  <si>
-    <t>Abordagem internacional para comparação</t>
-  </si>
-  <si>
-    <t>https://www.paho.org/pt/noticias/noticias-das-unidades-tecnicas</t>
-  </si>
-  <si>
-    <t>https://www.paho.org/pt/documentos-tecnicos-e-cientificos</t>
-  </si>
-  <si>
-    <t>Documentos técnicos e científicos</t>
-  </si>
-  <si>
-    <t>Saúde Pública Geral</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conteúdos atualizados, com diretrizes, estratégias e documentos operacionais que abrangem imunização, doenças crônicas, saúde mental, vetores, alimentação, trânsito e práticas clínicas. </t>
-  </si>
-  <si>
-    <t>https://www.paho.org/pt/publicacoes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Publicações </t>
-  </si>
-  <si>
-    <t>publicações e outros recursos informativos sobre os temas mais relevantes de saúde pública no continente americano.</t>
-  </si>
-  <si>
-    <t>https://www.gov.br/saude/pt-br/assuntos/saude-de-a-a-z</t>
-  </si>
-  <si>
-    <t>https://fiocruz.br/pesquisas-notas-tecnicas-e-relatorios</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov/health-topics.html#cdc-atozlist</t>
   </si>
   <si>
     <t>Nome do arquivo</t>
@@ -1322,16 +1198,8 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -1379,31 +1247,16 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1745,7 +1598,7 @@
   <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+      <selection activeCell="B1" sqref="B1:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1781,10 +1634,10 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>280</v>
+        <v>239</v>
       </c>
       <c r="I1" t="s">
-        <v>277</v>
+        <v>236</v>
       </c>
       <c r="J1" t="s">
         <v>7</v>
@@ -1806,17 +1659,17 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>406</v>
+        <v>365</v>
       </c>
       <c r="I2" t="s">
-        <v>278</v>
+        <v>237</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
@@ -1838,17 +1691,17 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>279</v>
+      <c r="F3" s="2" t="s">
+        <v>238</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>407</v>
+        <v>366</v>
       </c>
       <c r="I3" t="s">
-        <v>278</v>
+        <v>237</v>
       </c>
       <c r="J3" t="s">
         <v>13</v>
@@ -1870,17 +1723,17 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>408</v>
+        <v>367</v>
       </c>
       <c r="I4" t="s">
-        <v>281</v>
+        <v>240</v>
       </c>
       <c r="J4" t="s">
         <v>13</v>
@@ -1902,17 +1755,17 @@
       <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G5" t="s">
         <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>332</v>
+        <v>291</v>
       </c>
       <c r="I5" t="s">
-        <v>294</v>
+        <v>253</v>
       </c>
       <c r="J5" t="s">
         <v>22</v>
@@ -1934,17 +1787,17 @@
       <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G6" t="s">
         <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>345</v>
+        <v>304</v>
       </c>
       <c r="I6" t="s">
-        <v>346</v>
+        <v>305</v>
       </c>
       <c r="J6" t="s">
         <v>27</v>
@@ -1966,17 +1819,17 @@
       <c r="E7" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G7" t="s">
         <v>32</v>
       </c>
       <c r="H7" t="s">
-        <v>333</v>
+        <v>292</v>
       </c>
       <c r="I7" t="s">
-        <v>293</v>
+        <v>252</v>
       </c>
       <c r="J7" t="s">
         <v>33</v>
@@ -1998,17 +1851,17 @@
       <c r="E8" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G8" t="s">
         <v>37</v>
       </c>
       <c r="H8" t="s">
-        <v>347</v>
+        <v>306</v>
       </c>
       <c r="I8" t="s">
-        <v>348</v>
+        <v>307</v>
       </c>
       <c r="J8" t="s">
         <v>38</v>
@@ -2030,17 +1883,17 @@
       <c r="E9" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G9" t="s">
         <v>41</v>
       </c>
       <c r="H9" t="s">
-        <v>349</v>
+        <v>308</v>
       </c>
       <c r="I9" t="s">
-        <v>350</v>
+        <v>309</v>
       </c>
       <c r="J9" t="s">
         <v>42</v>
@@ -2051,7 +1904,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>344</v>
+        <v>303</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
@@ -2062,17 +1915,17 @@
       <c r="E10" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G10" t="s">
         <v>41</v>
       </c>
       <c r="H10" t="s">
-        <v>351</v>
+        <v>310</v>
       </c>
       <c r="I10" t="s">
-        <v>352</v>
+        <v>311</v>
       </c>
       <c r="J10" t="s">
         <v>45</v>
@@ -2094,17 +1947,17 @@
       <c r="E11" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G11" t="s">
         <v>41</v>
       </c>
       <c r="H11" t="s">
-        <v>353</v>
+        <v>312</v>
       </c>
       <c r="I11" t="s">
-        <v>354</v>
+        <v>313</v>
       </c>
       <c r="J11" t="s">
         <v>48</v>
@@ -2126,17 +1979,17 @@
       <c r="E12" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="2" t="s">
         <v>50</v>
       </c>
       <c r="G12" t="s">
         <v>41</v>
       </c>
       <c r="H12" t="s">
-        <v>355</v>
+        <v>314</v>
       </c>
       <c r="I12" t="s">
-        <v>356</v>
+        <v>315</v>
       </c>
       <c r="J12" t="s">
         <v>51</v>
@@ -2158,17 +2011,17 @@
       <c r="E13" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G13" t="s">
         <v>41</v>
       </c>
       <c r="H13" t="s">
-        <v>357</v>
+        <v>316</v>
       </c>
       <c r="I13" t="s">
-        <v>358</v>
+        <v>317</v>
       </c>
       <c r="J13" t="s">
         <v>55</v>
@@ -2190,17 +2043,17 @@
       <c r="E14" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="2" t="s">
         <v>57</v>
       </c>
       <c r="G14" t="s">
         <v>41</v>
       </c>
       <c r="H14" t="s">
-        <v>359</v>
+        <v>318</v>
       </c>
       <c r="I14" t="s">
-        <v>360</v>
+        <v>319</v>
       </c>
       <c r="J14" t="s">
         <v>58</v>
@@ -2222,17 +2075,17 @@
       <c r="E15" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="2" t="s">
         <v>61</v>
       </c>
       <c r="G15" t="s">
         <v>41</v>
       </c>
       <c r="H15" t="s">
-        <v>361</v>
+        <v>320</v>
       </c>
       <c r="I15" t="s">
-        <v>362</v>
+        <v>321</v>
       </c>
       <c r="J15" t="s">
         <v>62</v>
@@ -2254,17 +2107,17 @@
       <c r="E16" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="2" t="s">
         <v>64</v>
       </c>
       <c r="G16" t="s">
         <v>41</v>
       </c>
       <c r="H16" t="s">
-        <v>363</v>
+        <v>322</v>
       </c>
       <c r="I16" t="s">
-        <v>364</v>
+        <v>323</v>
       </c>
       <c r="J16" t="s">
         <v>65</v>
@@ -2286,17 +2139,17 @@
       <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="2" t="s">
         <v>67</v>
       </c>
       <c r="G17" t="s">
         <v>41</v>
       </c>
       <c r="H17" t="s">
-        <v>365</v>
+        <v>324</v>
       </c>
       <c r="I17" t="s">
-        <v>366</v>
+        <v>325</v>
       </c>
       <c r="J17" t="s">
         <v>68</v>
@@ -2318,17 +2171,17 @@
       <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G18" t="s">
         <v>41</v>
       </c>
       <c r="H18" t="s">
-        <v>367</v>
+        <v>326</v>
       </c>
       <c r="I18" t="s">
-        <v>368</v>
+        <v>327</v>
       </c>
       <c r="J18" t="s">
         <v>71</v>
@@ -2350,17 +2203,17 @@
       <c r="E19" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G19" t="s">
         <v>41</v>
       </c>
       <c r="H19" t="s">
-        <v>369</v>
+        <v>328</v>
       </c>
       <c r="I19" t="s">
-        <v>370</v>
+        <v>329</v>
       </c>
       <c r="J19" t="s">
         <v>74</v>
@@ -2376,23 +2229,23 @@
       <c r="C20" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="3">
         <v>45474</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G20" t="s">
         <v>77</v>
       </c>
       <c r="H20" t="s">
-        <v>334</v>
+        <v>293</v>
       </c>
       <c r="I20" t="s">
-        <v>295</v>
+        <v>254</v>
       </c>
       <c r="J20" t="s">
         <v>78</v>
@@ -2414,17 +2267,17 @@
       <c r="E21" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G21" t="s">
         <v>81</v>
       </c>
       <c r="H21" t="s">
-        <v>371</v>
+        <v>330</v>
       </c>
       <c r="I21" t="s">
-        <v>372</v>
+        <v>331</v>
       </c>
       <c r="J21" t="s">
         <v>82</v>
@@ -2446,17 +2299,17 @@
       <c r="E22" t="s">
         <v>84</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="2" t="s">
         <v>85</v>
       </c>
       <c r="G22" t="s">
         <v>41</v>
       </c>
       <c r="H22" t="s">
-        <v>373</v>
+        <v>332</v>
       </c>
       <c r="I22" t="s">
-        <v>374</v>
+        <v>333</v>
       </c>
       <c r="J22" t="s">
         <v>86</v>
@@ -2478,17 +2331,17 @@
       <c r="E23" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="2" t="s">
         <v>88</v>
       </c>
       <c r="G23" t="s">
         <v>41</v>
       </c>
       <c r="H23" t="s">
-        <v>375</v>
+        <v>334</v>
       </c>
       <c r="I23" t="s">
-        <v>376</v>
+        <v>335</v>
       </c>
       <c r="J23" t="s">
         <v>89</v>
@@ -2510,17 +2363,17 @@
       <c r="E24" t="s">
         <v>91</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="2" t="s">
         <v>92</v>
       </c>
       <c r="G24" t="s">
         <v>41</v>
       </c>
       <c r="H24" t="s">
-        <v>377</v>
+        <v>336</v>
       </c>
       <c r="I24" t="s">
-        <v>378</v>
+        <v>337</v>
       </c>
       <c r="J24" t="s">
         <v>93</v>
@@ -2542,17 +2395,17 @@
       <c r="E25" t="s">
         <v>95</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="2" t="s">
         <v>96</v>
       </c>
       <c r="G25" t="s">
         <v>97</v>
       </c>
       <c r="H25" t="s">
-        <v>379</v>
+        <v>338</v>
       </c>
       <c r="I25" t="s">
-        <v>380</v>
+        <v>339</v>
       </c>
       <c r="J25" t="s">
         <v>98</v>
@@ -2574,17 +2427,17 @@
       <c r="E26" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G26" t="s">
         <v>37</v>
       </c>
       <c r="H26" t="s">
-        <v>381</v>
+        <v>340</v>
       </c>
       <c r="I26" t="s">
-        <v>382</v>
+        <v>341</v>
       </c>
       <c r="J26" t="s">
         <v>101</v>
@@ -2606,17 +2459,17 @@
       <c r="E27" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="2" t="s">
         <v>103</v>
       </c>
       <c r="G27" t="s">
         <v>104</v>
       </c>
       <c r="H27" t="s">
-        <v>383</v>
+        <v>342</v>
       </c>
       <c r="I27" t="s">
-        <v>384</v>
+        <v>343</v>
       </c>
       <c r="J27" t="s">
         <v>105</v>
@@ -2638,17 +2491,17 @@
       <c r="E28" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="2" t="s">
         <v>107</v>
       </c>
       <c r="G28" t="s">
         <v>104</v>
       </c>
       <c r="H28" t="s">
-        <v>385</v>
+        <v>344</v>
       </c>
       <c r="I28" t="s">
-        <v>386</v>
+        <v>345</v>
       </c>
       <c r="J28" t="s">
         <v>108</v>
@@ -2670,17 +2523,17 @@
       <c r="E29" t="s">
         <v>10</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="2" t="s">
         <v>110</v>
       </c>
       <c r="G29" t="s">
         <v>104</v>
       </c>
       <c r="H29" t="s">
-        <v>335</v>
+        <v>294</v>
       </c>
       <c r="I29" t="s">
-        <v>296</v>
+        <v>255</v>
       </c>
       <c r="J29" t="s">
         <v>111</v>
@@ -2702,17 +2555,17 @@
       <c r="E30" t="s">
         <v>10</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="2" t="s">
         <v>113</v>
       </c>
       <c r="G30" t="s">
         <v>104</v>
       </c>
       <c r="H30" t="s">
-        <v>336</v>
+        <v>295</v>
       </c>
       <c r="I30" t="s">
-        <v>297</v>
+        <v>256</v>
       </c>
       <c r="J30" t="s">
         <v>114</v>
@@ -2734,17 +2587,17 @@
       <c r="E31" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="2" t="s">
         <v>116</v>
       </c>
       <c r="G31" t="s">
         <v>104</v>
       </c>
       <c r="H31" t="s">
-        <v>387</v>
+        <v>346</v>
       </c>
       <c r="I31" t="s">
-        <v>388</v>
+        <v>347</v>
       </c>
       <c r="J31" t="s">
         <v>117</v>
@@ -2766,17 +2619,17 @@
       <c r="E32" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G32" t="s">
         <v>104</v>
       </c>
       <c r="H32" t="s">
-        <v>409</v>
+        <v>368</v>
       </c>
       <c r="I32" t="s">
-        <v>284</v>
+        <v>243</v>
       </c>
       <c r="J32" t="s">
         <v>121</v>
@@ -2798,17 +2651,17 @@
       <c r="E33" t="s">
         <v>10</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="2" t="s">
         <v>123</v>
       </c>
       <c r="G33" t="s">
         <v>124</v>
       </c>
       <c r="H33" t="s">
-        <v>389</v>
+        <v>348</v>
       </c>
       <c r="I33" t="s">
-        <v>390</v>
+        <v>349</v>
       </c>
       <c r="J33" t="s">
         <v>125</v>
@@ -2830,17 +2683,17 @@
       <c r="E34" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="2" t="s">
         <v>127</v>
       </c>
       <c r="G34" t="s">
         <v>124</v>
       </c>
       <c r="H34" t="s">
-        <v>391</v>
+        <v>350</v>
       </c>
       <c r="I34" t="s">
-        <v>392</v>
+        <v>351</v>
       </c>
       <c r="J34" t="s">
         <v>128</v>
@@ -2862,17 +2715,17 @@
       <c r="E35" t="s">
         <v>10</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="2" t="s">
         <v>130</v>
       </c>
       <c r="G35" t="s">
         <v>131</v>
       </c>
       <c r="H35" t="s">
-        <v>410</v>
+        <v>369</v>
       </c>
       <c r="I35" t="s">
-        <v>282</v>
+        <v>241</v>
       </c>
       <c r="J35" t="s">
         <v>132</v>
@@ -2894,17 +2747,17 @@
       <c r="E36" t="s">
         <v>10</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" s="2" t="s">
         <v>134</v>
       </c>
       <c r="G36" t="s">
         <v>135</v>
       </c>
       <c r="H36" t="s">
-        <v>411</v>
+        <v>370</v>
       </c>
       <c r="I36" t="s">
-        <v>283</v>
+        <v>242</v>
       </c>
       <c r="J36" t="s">
         <v>136</v>
@@ -2926,17 +2779,17 @@
       <c r="E37" t="s">
         <v>10</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="2" t="s">
         <v>138</v>
       </c>
       <c r="G37" t="s">
         <v>139</v>
       </c>
       <c r="H37" t="s">
-        <v>393</v>
+        <v>352</v>
       </c>
       <c r="I37" t="s">
-        <v>394</v>
+        <v>353</v>
       </c>
       <c r="J37" t="s">
         <v>140</v>
@@ -2958,17 +2811,17 @@
       <c r="E38" t="s">
         <v>142</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="2" t="s">
         <v>143</v>
       </c>
       <c r="G38" t="s">
         <v>144</v>
       </c>
       <c r="H38" t="s">
-        <v>395</v>
+        <v>354</v>
       </c>
       <c r="I38" t="s">
-        <v>396</v>
+        <v>355</v>
       </c>
       <c r="J38" t="s">
         <v>145</v>
@@ -2979,7 +2832,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>299</v>
+        <v>258</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
@@ -2990,17 +2843,17 @@
       <c r="E39" t="s">
         <v>10</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F39" s="2" t="s">
         <v>147</v>
       </c>
       <c r="G39" t="s">
         <v>146</v>
       </c>
       <c r="H39" t="s">
-        <v>337</v>
+        <v>296</v>
       </c>
       <c r="I39" t="s">
-        <v>299</v>
+        <v>258</v>
       </c>
       <c r="J39" t="s">
         <v>148</v>
@@ -3011,7 +2864,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>300</v>
+        <v>259</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
@@ -3022,17 +2875,17 @@
       <c r="E40" t="s">
         <v>10</v>
       </c>
-      <c r="F40" s="7" t="s">
+      <c r="F40" s="2" t="s">
         <v>149</v>
       </c>
       <c r="G40" t="s">
         <v>150</v>
       </c>
       <c r="H40" t="s">
-        <v>338</v>
+        <v>297</v>
       </c>
       <c r="I40" t="s">
-        <v>301</v>
+        <v>260</v>
       </c>
       <c r="J40" t="s">
         <v>151</v>
@@ -3043,7 +2896,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>302</v>
+        <v>261</v>
       </c>
       <c r="C41" t="s">
         <v>18</v>
@@ -3054,17 +2907,17 @@
       <c r="E41" t="s">
         <v>10</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F41" s="2" t="s">
         <v>152</v>
       </c>
       <c r="G41" t="s">
         <v>150</v>
       </c>
       <c r="H41" t="s">
-        <v>339</v>
+        <v>298</v>
       </c>
       <c r="I41" t="s">
-        <v>303</v>
+        <v>262</v>
       </c>
       <c r="J41" t="s">
         <v>153</v>
@@ -3075,7 +2928,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>304</v>
+        <v>263</v>
       </c>
       <c r="C42" t="s">
         <v>18</v>
@@ -3093,10 +2946,10 @@
         <v>150</v>
       </c>
       <c r="H42" t="s">
-        <v>340</v>
+        <v>299</v>
       </c>
       <c r="I42" t="s">
-        <v>305</v>
+        <v>264</v>
       </c>
       <c r="J42" t="s">
         <v>155</v>
@@ -3118,17 +2971,17 @@
       <c r="E43" t="s">
         <v>10</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="F43" s="2" t="s">
         <v>158</v>
       </c>
       <c r="G43" t="s">
         <v>159</v>
       </c>
       <c r="H43" t="s">
-        <v>412</v>
+        <v>371</v>
       </c>
       <c r="I43" t="s">
-        <v>285</v>
+        <v>244</v>
       </c>
       <c r="J43" t="s">
         <v>160</v>
@@ -3150,17 +3003,17 @@
       <c r="E44" t="s">
         <v>10</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F44" s="2" t="s">
         <v>162</v>
       </c>
       <c r="G44" t="s">
         <v>163</v>
       </c>
       <c r="H44" t="s">
-        <v>397</v>
+        <v>356</v>
       </c>
       <c r="I44" t="s">
-        <v>398</v>
+        <v>357</v>
       </c>
       <c r="J44" t="s">
         <v>164</v>
@@ -3189,7 +3042,7 @@
         <v>163</v>
       </c>
       <c r="H45" t="s">
-        <v>399</v>
+        <v>358</v>
       </c>
       <c r="I45" t="s">
         <v>165</v>
@@ -3214,17 +3067,17 @@
       <c r="E46" t="s">
         <v>169</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="F46" s="2" t="s">
         <v>170</v>
       </c>
       <c r="G46" t="s">
         <v>171</v>
       </c>
       <c r="H46" t="s">
-        <v>413</v>
+        <v>372</v>
       </c>
       <c r="I46" t="s">
-        <v>286</v>
+        <v>245</v>
       </c>
       <c r="J46" t="s">
         <v>172</v>
@@ -3246,17 +3099,17 @@
       <c r="E47" t="s">
         <v>10</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="F47" s="2" t="s">
         <v>174</v>
       </c>
       <c r="G47" t="s">
         <v>175</v>
       </c>
       <c r="H47" t="s">
-        <v>414</v>
+        <v>373</v>
       </c>
       <c r="I47" t="s">
-        <v>287</v>
+        <v>246</v>
       </c>
       <c r="J47" t="s">
         <v>176</v>
@@ -3278,17 +3131,17 @@
       <c r="E48" t="s">
         <v>10</v>
       </c>
-      <c r="F48" s="7" t="s">
+      <c r="F48" s="2" t="s">
         <v>178</v>
       </c>
       <c r="G48" t="s">
         <v>179</v>
       </c>
       <c r="H48" t="s">
-        <v>415</v>
+        <v>374</v>
       </c>
       <c r="I48" t="s">
-        <v>289</v>
+        <v>248</v>
       </c>
       <c r="J48" t="s">
         <v>180</v>
@@ -3310,17 +3163,17 @@
       <c r="E49" t="s">
         <v>10</v>
       </c>
-      <c r="F49" s="7" t="s">
+      <c r="F49" s="2" t="s">
         <v>182</v>
       </c>
       <c r="G49" t="s">
         <v>183</v>
       </c>
       <c r="H49" t="s">
-        <v>416</v>
+        <v>375</v>
       </c>
       <c r="I49" t="s">
-        <v>288</v>
+        <v>247</v>
       </c>
       <c r="J49" t="s">
         <v>184</v>
@@ -3342,17 +3195,17 @@
       <c r="E50" t="s">
         <v>186</v>
       </c>
-      <c r="F50" s="7" t="s">
+      <c r="F50" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G50" t="s">
         <v>188</v>
       </c>
       <c r="H50" t="s">
-        <v>417</v>
+        <v>376</v>
       </c>
       <c r="I50" t="s">
-        <v>290</v>
+        <v>249</v>
       </c>
       <c r="J50" t="s">
         <v>189</v>
@@ -3374,17 +3227,17 @@
       <c r="E51" t="s">
         <v>191</v>
       </c>
-      <c r="F51" s="7" t="s">
+      <c r="F51" s="2" t="s">
         <v>192</v>
       </c>
       <c r="G51" t="s">
         <v>193</v>
       </c>
       <c r="H51" t="s">
-        <v>400</v>
+        <v>359</v>
       </c>
       <c r="I51" t="s">
-        <v>401</v>
+        <v>360</v>
       </c>
       <c r="J51" t="s">
         <v>194</v>
@@ -3395,7 +3248,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>306</v>
+        <v>265</v>
       </c>
       <c r="C52" t="s">
         <v>18</v>
@@ -3406,17 +3259,17 @@
       <c r="E52" t="s">
         <v>10</v>
       </c>
-      <c r="F52" s="7" t="s">
+      <c r="F52" s="2" t="s">
         <v>195</v>
       </c>
       <c r="G52" t="s">
         <v>188</v>
       </c>
       <c r="H52" t="s">
-        <v>341</v>
+        <v>300</v>
       </c>
       <c r="I52" t="s">
-        <v>307</v>
+        <v>266</v>
       </c>
       <c r="J52" t="s">
         <v>196</v>
@@ -3427,7 +3280,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>308</v>
+        <v>267</v>
       </c>
       <c r="C53" t="s">
         <v>18</v>
@@ -3438,17 +3291,17 @@
       <c r="E53" t="s">
         <v>10</v>
       </c>
-      <c r="F53" s="7" t="s">
+      <c r="F53" s="2" t="s">
         <v>197</v>
       </c>
       <c r="G53" t="s">
         <v>198</v>
       </c>
       <c r="H53" t="s">
-        <v>342</v>
+        <v>301</v>
       </c>
       <c r="I53" t="s">
-        <v>309</v>
+        <v>268</v>
       </c>
       <c r="J53" t="s">
         <v>199</v>
@@ -3459,7 +3312,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>310</v>
+        <v>269</v>
       </c>
       <c r="C54" t="s">
         <v>18</v>
@@ -3470,17 +3323,17 @@
       <c r="E54" t="s">
         <v>10</v>
       </c>
-      <c r="F54" s="7" t="s">
+      <c r="F54" s="2" t="s">
         <v>200</v>
       </c>
       <c r="G54" t="s">
         <v>201</v>
       </c>
       <c r="H54" t="s">
-        <v>343</v>
+        <v>302</v>
       </c>
       <c r="I54" t="s">
-        <v>311</v>
+        <v>270</v>
       </c>
       <c r="J54" t="s">
         <v>202</v>
@@ -3491,7 +3344,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>312</v>
+        <v>271</v>
       </c>
       <c r="C55" t="s">
         <v>18</v>
@@ -3502,17 +3355,17 @@
       <c r="E55" t="s">
         <v>10</v>
       </c>
-      <c r="F55" s="7" t="s">
+      <c r="F55" s="2" t="s">
         <v>203</v>
       </c>
       <c r="G55" t="s">
         <v>201</v>
       </c>
       <c r="H55" t="s">
-        <v>313</v>
+        <v>272</v>
       </c>
       <c r="I55" t="s">
-        <v>314</v>
+        <v>273</v>
       </c>
       <c r="J55" t="s">
         <v>204</v>
@@ -3522,8 +3375,8 @@
       <c r="A56">
         <v>56</v>
       </c>
-      <c r="B56" s="9" t="s">
-        <v>315</v>
+      <c r="B56" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="C56" t="s">
         <v>18</v>
@@ -3534,17 +3387,17 @@
       <c r="E56" t="s">
         <v>10</v>
       </c>
-      <c r="F56" s="7" t="s">
+      <c r="F56" s="2" t="s">
         <v>205</v>
       </c>
       <c r="G56" t="s">
         <v>201</v>
       </c>
       <c r="H56" t="s">
-        <v>316</v>
+        <v>275</v>
       </c>
       <c r="I56" t="s">
-        <v>317</v>
+        <v>276</v>
       </c>
       <c r="J56" t="s">
         <v>206</v>
@@ -3566,17 +3419,17 @@
       <c r="E57" t="s">
         <v>10</v>
       </c>
-      <c r="F57" s="7" t="s">
+      <c r="F57" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G57" t="s">
         <v>201</v>
       </c>
       <c r="H57" t="s">
-        <v>402</v>
+        <v>361</v>
       </c>
       <c r="I57" t="s">
-        <v>403</v>
+        <v>362</v>
       </c>
       <c r="J57" t="s">
         <v>209</v>
@@ -3587,7 +3440,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>318</v>
+        <v>277</v>
       </c>
       <c r="C58" t="s">
         <v>18</v>
@@ -3598,17 +3451,17 @@
       <c r="E58" t="s">
         <v>10</v>
       </c>
-      <c r="F58" s="7" t="s">
+      <c r="F58" s="2" t="s">
         <v>210</v>
       </c>
       <c r="G58" t="s">
         <v>211</v>
       </c>
       <c r="H58" t="s">
-        <v>319</v>
+        <v>278</v>
       </c>
       <c r="I58" t="s">
-        <v>320</v>
+        <v>279</v>
       </c>
       <c r="J58" t="s">
         <v>212</v>
@@ -3619,7 +3472,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>321</v>
+        <v>280</v>
       </c>
       <c r="C59" t="s">
         <v>18</v>
@@ -3630,17 +3483,17 @@
       <c r="E59" t="s">
         <v>10</v>
       </c>
-      <c r="F59" s="7" t="s">
+      <c r="F59" s="2" t="s">
         <v>213</v>
       </c>
       <c r="G59" t="s">
         <v>211</v>
       </c>
       <c r="H59" t="s">
-        <v>322</v>
+        <v>281</v>
       </c>
       <c r="I59" t="s">
-        <v>323</v>
+        <v>282</v>
       </c>
       <c r="J59" t="s">
         <v>214</v>
@@ -3650,8 +3503,8 @@
       <c r="A60">
         <v>60</v>
       </c>
-      <c r="B60" s="10" t="s">
-        <v>298</v>
+      <c r="B60" s="5" t="s">
+        <v>257</v>
       </c>
       <c r="C60" t="s">
         <v>18</v>
@@ -3662,17 +3515,17 @@
       <c r="E60" t="s">
         <v>215</v>
       </c>
-      <c r="F60" s="7" t="s">
+      <c r="F60" s="2" t="s">
         <v>216</v>
       </c>
       <c r="G60" t="s">
         <v>217</v>
       </c>
       <c r="H60" t="s">
-        <v>324</v>
+        <v>283</v>
       </c>
       <c r="I60" t="s">
-        <v>325</v>
+        <v>284</v>
       </c>
       <c r="J60" t="s">
         <v>218</v>
@@ -3694,17 +3547,17 @@
       <c r="E61" t="s">
         <v>10</v>
       </c>
-      <c r="F61" s="7" t="s">
+      <c r="F61" s="2" t="s">
         <v>220</v>
       </c>
       <c r="G61" t="s">
         <v>221</v>
       </c>
       <c r="H61" t="s">
-        <v>404</v>
+        <v>363</v>
       </c>
       <c r="I61" t="s">
-        <v>405</v>
+        <v>364</v>
       </c>
       <c r="J61" t="s">
         <v>222</v>
@@ -3726,17 +3579,17 @@
       <c r="E62" t="s">
         <v>10</v>
       </c>
-      <c r="F62" s="7" t="s">
+      <c r="F62" s="2" t="s">
         <v>224</v>
       </c>
       <c r="G62" t="s">
         <v>221</v>
       </c>
       <c r="H62" t="s">
-        <v>418</v>
+        <v>377</v>
       </c>
       <c r="I62" t="s">
-        <v>291</v>
+        <v>250</v>
       </c>
       <c r="J62" t="s">
         <v>225</v>
@@ -3746,8 +3599,8 @@
       <c r="A63">
         <v>63</v>
       </c>
-      <c r="B63" s="9" t="s">
-        <v>326</v>
+      <c r="B63" s="4" t="s">
+        <v>285</v>
       </c>
       <c r="C63" t="s">
         <v>18</v>
@@ -3758,17 +3611,17 @@
       <c r="E63" t="s">
         <v>10</v>
       </c>
-      <c r="F63" s="7" t="s">
+      <c r="F63" s="2" t="s">
         <v>226</v>
       </c>
       <c r="G63" t="s">
         <v>227</v>
       </c>
       <c r="H63" t="s">
-        <v>327</v>
+        <v>286</v>
       </c>
       <c r="I63" t="s">
-        <v>328</v>
+        <v>287</v>
       </c>
       <c r="J63" t="s">
         <v>228</v>
@@ -3779,7 +3632,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>329</v>
+        <v>288</v>
       </c>
       <c r="C64" t="s">
         <v>18</v>
@@ -3790,17 +3643,17 @@
       <c r="E64" t="s">
         <v>10</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F64" s="2" t="s">
         <v>229</v>
       </c>
       <c r="G64" t="s">
         <v>230</v>
       </c>
       <c r="H64" t="s">
-        <v>330</v>
+        <v>289</v>
       </c>
       <c r="I64" t="s">
-        <v>331</v>
+        <v>290</v>
       </c>
       <c r="J64" t="s">
         <v>231</v>
@@ -3822,17 +3675,17 @@
       <c r="E65" t="s">
         <v>10</v>
       </c>
-      <c r="F65" s="7" t="s">
+      <c r="F65" s="2" t="s">
         <v>233</v>
       </c>
       <c r="G65" t="s">
         <v>234</v>
       </c>
       <c r="H65" t="s">
-        <v>419</v>
+        <v>378</v>
       </c>
       <c r="I65" t="s">
-        <v>292</v>
+        <v>251</v>
       </c>
       <c r="J65" t="s">
         <v>235</v>
@@ -3906,196 +3759,4 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C878AD0-DA59-4B8E-B1DC-CCBDB4F7325E}">
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="23.44140625" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" customWidth="1"/>
-    <col min="6" max="6" width="61.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="144" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{A92B9505-7886-4ED7-9639-7E0ECF7B2A60}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{58763747-0B5A-4670-BD7D-AC28D26E7EA6}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{9D1EA300-5E47-420C-867E-D74DCE23C87D}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{79098094-975F-4C37-A45B-98E79FB1301A}"/>
-    <hyperlink ref="B7" r:id="rId5" xr:uid="{9F537745-A0EE-4649-9086-36378DA48E7D}"/>
-    <hyperlink ref="B8" r:id="rId6" location="cdc-atozlist" xr:uid="{1A0E18FD-62AC-42A9-AD3A-515367689A09}"/>
-    <hyperlink ref="B2" r:id="rId7" xr:uid="{1B06AA73-66D5-4867-BB6A-8D59D351C21D}"/>
-  </hyperlinks>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
novos arquivos e script da etapa 4
</commit_message>
<xml_diff>
--- a/controle_documentos.xlsx
+++ b/controle_documentos.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isisi\Documents\IAVS_PROJETO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB21F8A7-9D54-47FC-8551-0E6CC1708FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D65BCB9-7D91-4F22-8848-2A263A6F9B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7495ED94-32AF-4984-90A6-A4DB1F4E4893}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7495ED94-32AF-4984-90A6-A4DB1F4E4893}"/>
   </bookViews>
   <sheets>
     <sheet name="docs" sheetId="2" r:id="rId1"/>
+    <sheet name="fontes_complementares" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">docs!$A$1:$J$65</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="420">
   <si>
     <t>ID</t>
   </si>
@@ -1189,6 +1190,129 @@
   </si>
   <si>
     <t>C:\Users\isisi\Documents\IAVS_PROJETO\manuais\manual-tecnico-para-o-diagnostico-da-sifilis.pdf</t>
+  </si>
+  <si>
+    <t>Conteúdo Útil</t>
+  </si>
+  <si>
+    <t>Doenças/Tema</t>
+  </si>
+  <si>
+    <t>Observações</t>
+  </si>
+  <si>
+    <t>OPAS/OMS</t>
+  </si>
+  <si>
+    <t>https://www.paho.org/pt/documentos-tecnicos-e-cientificos</t>
+  </si>
+  <si>
+    <t>Documentos técnicos e científicos</t>
+  </si>
+  <si>
+    <t>Atualizações frequentes sobre surtos, novas recomendações técnicas</t>
+  </si>
+  <si>
+    <t>Saúde Pública Geral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conteúdos atualizados, com diretrizes, estratégias e documentos operacionais que abrangem imunização, doenças crônicas, saúde mental, vetores, alimentação, trânsito e práticas clínicas. </t>
+  </si>
+  <si>
+    <t>https://www.paho.org/pt/noticias/noticias-das-unidades-tecnicas</t>
+  </si>
+  <si>
+    <t>Notícias Técnicas</t>
+  </si>
+  <si>
+    <t>Diversas doenças emergentes</t>
+  </si>
+  <si>
+    <t>Boletins com abordagem técnica e operacional</t>
+  </si>
+  <si>
+    <t>https://www.paho.org/pt/publicacoes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publicações </t>
+  </si>
+  <si>
+    <t>publicações e outros recursos informativos sobre os temas mais relevantes de saúde pública no continente americano.</t>
+  </si>
+  <si>
+    <t>Pode conter atualizações de protocolos</t>
+  </si>
+  <si>
+    <t>Ministério da Saúde</t>
+  </si>
+  <si>
+    <t>https://www.gov.br/saude/pt-br/assuntos/saude-de-a-a-z</t>
+  </si>
+  <si>
+    <t>Portal por doenças</t>
+  </si>
+  <si>
+    <t>Links diretos por ordem alfabética de temas</t>
+  </si>
+  <si>
+    <t>Zoonoses, arboviroses, HIV, etc.</t>
+  </si>
+  <si>
+    <t>Acesso rápido a documentos específicos por tema</t>
+  </si>
+  <si>
+    <t>Anvisa</t>
+  </si>
+  <si>
+    <t>https://www.gov.br/anvisa/pt-br/assuntos/noticias-anvisa</t>
+  </si>
+  <si>
+    <t>Notícias Regulatórias</t>
+  </si>
+  <si>
+    <t>Alertas e novas orientações sobre medicamentos e vigilância sanitária</t>
+  </si>
+  <si>
+    <t>Segurança do paciente, surtos</t>
+  </si>
+  <si>
+    <t>Conteúdo dinâmico e complementar</t>
+  </si>
+  <si>
+    <t>Fiocruz</t>
+  </si>
+  <si>
+    <t>https://fiocruz.br/pesquisas-notas-tecnicas-e-relatorios</t>
+  </si>
+  <si>
+    <t>Publicações Técnicas</t>
+  </si>
+  <si>
+    <t>Guias, recomendações e estudos técnicos</t>
+  </si>
+  <si>
+    <t>Saúde Pública em geral</t>
+  </si>
+  <si>
+    <t>Produções recentes que não estão listadas nos seus PDFs</t>
+  </si>
+  <si>
+    <t>CDC</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov/health-topics.html#cdc-atozlist</t>
+  </si>
+  <si>
+    <t>Conteúdo Técnico</t>
+  </si>
+  <si>
+    <t>Protocolos e fichas técnicas por doença</t>
+  </si>
+  <si>
+    <t>Dengue, Influenza, etc.</t>
+  </si>
+  <si>
+    <t>Abordagem internacional para comparação</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1322,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1227,6 +1351,14 @@
       <name val="Aptos"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1250,7 +1382,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1258,6 +1390,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1597,8 +1744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{919F2911-7189-4630-87F2-2D10037DF89A}">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:M7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3759,4 +3906,196 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E433BF9F-D624-43EA-B05A-9638B55985E0}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" customWidth="1"/>
+    <col min="6" max="6" width="61.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>419</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{693D012F-D454-404E-950F-D6EAE0CFDD9A}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{91BC1500-C11D-40FF-87A6-68EF22A93E36}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{1145CACC-386D-417E-BDEA-763EF03E35FE}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{357C14ED-27F0-4882-8DFE-25FA13D58F16}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{E046CAEC-18DE-4CE2-BE99-D20F4AAD112B}"/>
+    <hyperlink ref="B8" r:id="rId6" location="cdc-atozlist" xr:uid="{B94E372D-4F5F-41F6-8708-3D96B4586EB0}"/>
+    <hyperlink ref="B2" r:id="rId7" xr:uid="{31B26AEA-F6AD-4509-93DF-6491787D0937}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>